<commit_message>
mods for data processing to work with FM
</commit_message>
<xml_diff>
--- a/cal/Test_Repo/AsRun.xlsx
+++ b/cal/Test_Repo/AsRun.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonny Woof\Google Drive\Python_packages_woof\pyMAP\cal\Test_Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E6CA08-23E7-468D-824C-78D18DB676B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8453C50-97CF-4989-A211-ED0463E05908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="603" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="603" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="252">
   <si>
     <t>Calibration Procedure Reference</t>
   </si>
@@ -809,6 +809,18 @@
   </si>
   <si>
     <t>Sensor Elevation [deg]  (+2:bottom, 0:middle, -2:top) (+2,0,-2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABM Doubles rate [Cts/Sec] </t>
+  </si>
+  <si>
+    <t>PSPL_abm_cnt</t>
+  </si>
+  <si>
+    <t>Beam Enabled</t>
+  </si>
+  <si>
+    <t>beamEnabled</t>
   </si>
 </sst>
 </file>
@@ -2154,110 +2166,6 @@
   </cellStyles>
   <dxfs count="169">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <vertical/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2346,6 +2254,110 @@
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <vertical/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -3013,26 +3025,26 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{50969DF8-9268-4F4F-83BF-D77B96DFE259}" name="Table757" displayName="Table757" ref="E3:U100" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{50969DF8-9268-4F4F-83BF-D77B96DFE259}" name="Table757" displayName="Table757" ref="E3:U100" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="E3:U100" xr:uid="{3A6D676D-E199-4A43-BB30-06E91BA25197}"/>
   <tableColumns count="17">
-    <tableColumn id="26" xr3:uid="{BC44A319-D44C-4ACA-B406-C469B26CDCBD}" name="str_ap_mm" dataDxfId="37"/>
-    <tableColumn id="32" xr3:uid="{E947E291-9DB3-4F3E-9A25-394CB4E00106}" name="str_mag" dataDxfId="36"/>
-    <tableColumn id="28" xr3:uid="{5F8894E8-1849-403F-BB92-0AE405681005}" name="str_wave12" dataDxfId="35"/>
-    <tableColumn id="27" xr3:uid="{42729D3F-FEC4-4A7E-98B7-0BC5E4D9CDC6}" name="str_wave2" dataDxfId="34"/>
-    <tableColumn id="24" xr3:uid="{57E7BC4A-2D54-45AE-940B-D1DDCC03F282}" name="str_specIrrad" dataDxfId="33"/>
-    <tableColumn id="23" xr3:uid="{3AC76F7A-DB05-44E5-AED2-37315286A787}" name="str_specRad" dataDxfId="32"/>
-    <tableColumn id="22" xr3:uid="{E48D7AFF-FA3E-4456-BD54-1399C27298FF}" name="str_v" dataDxfId="31"/>
-    <tableColumn id="21" xr3:uid="{314CC932-FCE2-4858-8600-DCF744C1BD1B}" name="str_azm" dataDxfId="30"/>
-    <tableColumn id="20" xr3:uid="{40095607-F028-4D1C-BDE4-E8A084989267}" name="str_elv" dataDxfId="29"/>
-    <tableColumn id="19" xr3:uid="{D912C668-1B72-4EDC-A091-35936ACBCF11}" name="str_amp" dataDxfId="28"/>
-    <tableColumn id="18" xr3:uid="{95AD5FCF-2275-4E73-A103-980B932A4C52}" name="str_scan" dataDxfId="27"/>
-    <tableColumn id="29" xr3:uid="{2E08C0CA-1625-4F5C-BC79-BFA3D3E3FDF9}" name="str_scanStart" dataDxfId="26"/>
-    <tableColumn id="30" xr3:uid="{05DBA09C-694F-4658-B497-214629D69633}" name="str_scanStop" dataDxfId="25"/>
-    <tableColumn id="1" xr3:uid="{8666DA5C-492C-41C4-BB8C-9DD00FFC6D46}" name="str_scanStep" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{A864E2F6-AAA6-459A-8F53-32959EA036A3}" name="str_scanDelay" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{7B041EE5-2479-4638-8688-B6D0E937010E}" name="str_scanInterval" dataDxfId="22"/>
-    <tableColumn id="13" xr3:uid="{92F3D1B2-3899-4CCB-93E0-62D4B2772BB5}" name="str_filename" dataDxfId="21"/>
+    <tableColumn id="26" xr3:uid="{BC44A319-D44C-4ACA-B406-C469B26CDCBD}" name="str_ap_mm" dataDxfId="16"/>
+    <tableColumn id="32" xr3:uid="{E947E291-9DB3-4F3E-9A25-394CB4E00106}" name="str_mag" dataDxfId="15"/>
+    <tableColumn id="28" xr3:uid="{5F8894E8-1849-403F-BB92-0AE405681005}" name="str_wave12" dataDxfId="14"/>
+    <tableColumn id="27" xr3:uid="{42729D3F-FEC4-4A7E-98B7-0BC5E4D9CDC6}" name="str_wave2" dataDxfId="13"/>
+    <tableColumn id="24" xr3:uid="{57E7BC4A-2D54-45AE-940B-D1DDCC03F282}" name="str_specIrrad" dataDxfId="12"/>
+    <tableColumn id="23" xr3:uid="{3AC76F7A-DB05-44E5-AED2-37315286A787}" name="str_specRad" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{E48D7AFF-FA3E-4456-BD54-1399C27298FF}" name="str_v" dataDxfId="10"/>
+    <tableColumn id="21" xr3:uid="{314CC932-FCE2-4858-8600-DCF744C1BD1B}" name="str_azm" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{40095607-F028-4D1C-BDE4-E8A084989267}" name="str_elv" dataDxfId="8"/>
+    <tableColumn id="19" xr3:uid="{D912C668-1B72-4EDC-A091-35936ACBCF11}" name="str_amp" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{95AD5FCF-2275-4E73-A103-980B932A4C52}" name="str_scan" dataDxfId="6"/>
+    <tableColumn id="29" xr3:uid="{2E08C0CA-1625-4F5C-BC79-BFA3D3E3FDF9}" name="str_scanStart" dataDxfId="5"/>
+    <tableColumn id="30" xr3:uid="{05DBA09C-694F-4658-B497-214629D69633}" name="str_scanStop" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{8666DA5C-492C-41C4-BB8C-9DD00FFC6D46}" name="str_scanStep" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{A864E2F6-AAA6-459A-8F53-32959EA036A3}" name="str_scanDelay" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{7B041EE5-2479-4638-8688-B6D0E937010E}" name="str_scanInterval" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{92F3D1B2-3899-4CCB-93E0-62D4B2772BB5}" name="str_filename" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3185,49 +3197,49 @@
     <tableColumn id="20" xr3:uid="{386DD8CB-78BE-410A-8DC1-73D1ED742FB9}" name="beamPy" dataDxfId="50"/>
     <tableColumn id="19" xr3:uid="{354F813E-FB09-4A34-A497-A34D088A8DC9}" name="beamISpress" dataDxfId="49"/>
     <tableColumn id="18" xr3:uid="{6454750B-7285-4FD6-A50C-922F20AD9E31}" name="sourcePress" dataDxfId="48"/>
-    <tableColumn id="29" xr3:uid="{E070A16B-A0AA-4B33-8CCB-BB56FAB972D9}" name="pressureBeam" dataDxfId="47"/>
+    <tableColumn id="29" xr3:uid="{E070A16B-A0AA-4B33-8CCB-BB56FAB972D9}" name="beamEnabled" dataDxfId="47"/>
     <tableColumn id="30" xr3:uid="{DC2B29F4-AF6A-4E39-ABE0-3B6B4FE3B114}" name="pressureChamber" dataDxfId="46"/>
     <tableColumn id="1" xr3:uid="{E3D91A3D-E113-45A2-A922-6668EC7CA58F}" name="chamber_ig" dataDxfId="45"/>
     <tableColumn id="12" xr3:uid="{08DC4079-F56E-4074-BF0E-CED3980C8DC7}" name="stageOuter" dataDxfId="44"/>
     <tableColumn id="13" xr3:uid="{2F2983A7-407F-4EDF-8BC1-138DE21A3157}" name="stageInner" dataDxfId="43"/>
     <tableColumn id="14" xr3:uid="{7255253D-A80B-427D-851F-23EA2CCEBA6A}" name="stageX" dataDxfId="42"/>
-    <tableColumn id="25" xr3:uid="{B262986D-F56B-4D6E-896C-71DCF93C0686}" name="PSPL_seq" dataDxfId="41"/>
+    <tableColumn id="25" xr3:uid="{B262986D-F56B-4D6E-896C-71DCF93C0686}" name="PSPL_abm_cnt" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6F93FEA6-A539-40E7-A221-6BDC4CEA6272}" name="Table7511" displayName="Table7511" ref="E3:V100" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6F93FEA6-A539-40E7-A221-6BDC4CEA6272}" name="Table7511" displayName="Table7511" ref="E3:V100" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="E3:V100" xr:uid="{3A6D676D-E199-4A43-BB30-06E91BA25197}"/>
   <tableColumns count="18">
-    <tableColumn id="26" xr3:uid="{101434C2-96CA-40FB-8866-A99DBB13D1E1}" name="gas" dataDxfId="17"/>
-    <tableColumn id="32" xr3:uid="{369D796D-5396-4EA1-B4AE-92B67652F806}" name="species" dataDxfId="16"/>
-    <tableColumn id="28" xr3:uid="{7392B926-F4D1-4C0E-826E-18286A72421A}" name="beam_ke" dataDxfId="15"/>
-    <tableColumn id="27" xr3:uid="{B5024841-48BA-4D98-9AF7-A2DDFD8301C2}" name="I_emm" dataDxfId="14"/>
-    <tableColumn id="24" xr3:uid="{AE9E4E69-67F5-498C-9DA5-F86B9D4642D6}" name="voltFocus1" dataDxfId="13"/>
-    <tableColumn id="23" xr3:uid="{5501A29A-CA07-4642-93DC-5FDA4CCF838B}" name="voltFocus2" dataDxfId="12"/>
-    <tableColumn id="22" xr3:uid="{BD698434-97D6-4793-9AD9-78FC0DA223EC}" name="beamKe" dataDxfId="11"/>
-    <tableColumn id="21" xr3:uid="{99A047C8-DFF4-4237-9B72-F2403E154A33}" name="beamPx" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{D5BABF1F-CF05-4C68-B962-BAE710D876D1}" name="beamPy" dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{C058E913-2F9A-4B04-87F3-89E202A16CA9}" name="beamISpress" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{09F2B301-876D-4185-B311-E0017ADC05D4}" name="sourcePress" dataDxfId="7"/>
-    <tableColumn id="29" xr3:uid="{F5C09295-6CD2-445D-B2BE-C01D799FBAA2}" name="pressureBeam" dataDxfId="6"/>
-    <tableColumn id="30" xr3:uid="{77B1F785-95A5-483C-96FC-EB636E31B473}" name="pressureChamber" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{BBA9C4DD-4EF2-4E01-9EA1-E7D2F32032FF}" name="chamber_ig" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{4B02803C-1F28-4E43-947F-E046AC389332}" name="stageOuter" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{FD63BB10-2FB6-4735-942D-329696C612A2}" name="stageInner" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{22D297A3-AE91-4F11-9152-7CAFE98C760D}" name="stageX" dataDxfId="1"/>
-    <tableColumn id="25" xr3:uid="{1FE4B1F3-29DD-4E99-B889-01F9CF5B449D}" name="PSPL_seq" dataDxfId="0"/>
+    <tableColumn id="26" xr3:uid="{101434C2-96CA-40FB-8866-A99DBB13D1E1}" name="gas" dataDxfId="37"/>
+    <tableColumn id="32" xr3:uid="{369D796D-5396-4EA1-B4AE-92B67652F806}" name="species" dataDxfId="36"/>
+    <tableColumn id="28" xr3:uid="{7392B926-F4D1-4C0E-826E-18286A72421A}" name="beam_ke" dataDxfId="35"/>
+    <tableColumn id="27" xr3:uid="{B5024841-48BA-4D98-9AF7-A2DDFD8301C2}" name="I_emm" dataDxfId="34"/>
+    <tableColumn id="24" xr3:uid="{AE9E4E69-67F5-498C-9DA5-F86B9D4642D6}" name="voltFocus1" dataDxfId="33"/>
+    <tableColumn id="23" xr3:uid="{5501A29A-CA07-4642-93DC-5FDA4CCF838B}" name="voltFocus2" dataDxfId="32"/>
+    <tableColumn id="22" xr3:uid="{BD698434-97D6-4793-9AD9-78FC0DA223EC}" name="beamKe" dataDxfId="31"/>
+    <tableColumn id="21" xr3:uid="{99A047C8-DFF4-4237-9B72-F2403E154A33}" name="beamPx" dataDxfId="30"/>
+    <tableColumn id="20" xr3:uid="{D5BABF1F-CF05-4C68-B962-BAE710D876D1}" name="beamPy" dataDxfId="29"/>
+    <tableColumn id="19" xr3:uid="{C058E913-2F9A-4B04-87F3-89E202A16CA9}" name="beamISpress" dataDxfId="28"/>
+    <tableColumn id="18" xr3:uid="{09F2B301-876D-4185-B311-E0017ADC05D4}" name="sourcePress" dataDxfId="27"/>
+    <tableColumn id="29" xr3:uid="{F5C09295-6CD2-445D-B2BE-C01D799FBAA2}" name="pressureBeam" dataDxfId="26"/>
+    <tableColumn id="30" xr3:uid="{77B1F785-95A5-483C-96FC-EB636E31B473}" name="pressureChamber" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{BBA9C4DD-4EF2-4E01-9EA1-E7D2F32032FF}" name="chamber_ig" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{4B02803C-1F28-4E43-947F-E046AC389332}" name="stageOuter" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{FD63BB10-2FB6-4735-942D-329696C612A2}" name="stageInner" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{22D297A3-AE91-4F11-9152-7CAFE98C760D}" name="stageX" dataDxfId="21"/>
+    <tableColumn id="25" xr3:uid="{1FE4B1F3-29DD-4E99-B889-01F9CF5B449D}" name="PSPL_seq" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3265,7 +3277,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3371,7 +3383,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3513,7 +3525,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -36606,8 +36618,8 @@
   <dimension ref="A1:V406"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="F1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="W1" sqref="W1"/>
+      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44087,8 +44099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FC9A05-C9E5-4DD5-85DD-15F69BF3EEE3}">
   <dimension ref="A1:V406"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44203,7 +44215,7 @@
         <v>186</v>
       </c>
       <c r="P2" s="122" t="s">
-        <v>70</v>
+        <v>250</v>
       </c>
       <c r="Q2" s="11" t="s">
         <v>71</v>
@@ -44221,7 +44233,7 @@
         <v>200</v>
       </c>
       <c r="V2" s="43" t="s">
-        <v>41</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -44275,7 +44287,7 @@
         <v>195</v>
       </c>
       <c r="P3" s="123" t="s">
-        <v>206</v>
+        <v>251</v>
       </c>
       <c r="Q3" s="17" t="s">
         <v>207</v>
@@ -44293,7 +44305,7 @@
         <v>203</v>
       </c>
       <c r="V3" s="44" t="s">
-        <v>196</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -51724,7 +51736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329974D5-2AFB-445C-B663-67C7FECFDBD8}">
   <dimension ref="A1:V406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>

</xml_diff>